<commit_message>
service test  import data to database success
</commit_message>
<xml_diff>
--- a/doc/log/log_201508030314_chaixiaoyin.xlsx
+++ b/doc/log/log_201508030314_chaixiaoyin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15825" windowHeight="4965"/>
+    <workbookView windowWidth="21120" windowHeight="6660"/>
   </bookViews>
   <sheets>
     <sheet name="日志" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38">
   <si>
     <t>日期</t>
   </si>
@@ -122,6 +122,15 @@
   </si>
   <si>
     <t>对dao和service进行调试</t>
+  </si>
+  <si>
+    <t>service测试可以运行</t>
+  </si>
+  <si>
+    <t>9:00-11:00</t>
+  </si>
+  <si>
+    <t>对web进行补充和测试</t>
   </si>
   <si>
     <t>周次</t>
@@ -135,8 +144,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -149,47 +158,99 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -203,59 +264,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -264,23 +272,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,19 +311,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -326,55 +455,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -386,103 +467,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,6 +502,47 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -511,17 +561,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -544,50 +597,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -599,10 +608,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -611,133 +620,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1079,7 +1088,7 @@
   <sheetPr/>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1273,14 +1282,24 @@
       <c r="C11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="A12" s="1">
+        <v>43256</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="4"/>
@@ -1340,13 +1359,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
update main for   web
</commit_message>
<xml_diff>
--- a/doc/log/log_201508030314_chaixiaoyin.xlsx
+++ b/doc/log/log_201508030314_chaixiaoyin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21120" windowHeight="6660"/>
+    <workbookView windowWidth="11940" windowHeight="6525"/>
   </bookViews>
   <sheets>
     <sheet name="日志" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41">
   <si>
     <t>日期</t>
   </si>
@@ -131,6 +131,15 @@
   </si>
   <si>
     <t>对web进行补充和测试</t>
+  </si>
+  <si>
+    <t>测试失败</t>
+  </si>
+  <si>
+    <t>18:00-19:00</t>
+  </si>
+  <si>
+    <t>对web进行分析</t>
   </si>
   <si>
     <t>周次</t>
@@ -158,6 +167,142 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -165,142 +310,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -311,78 +320,162 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -395,7 +488,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,90 +501,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,6 +511,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -522,59 +546,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -597,8 +571,43 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -608,10 +617,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -620,133 +629,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1089,7 +1098,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
@@ -1300,14 +1309,22 @@
       <c r="C12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="A13" s="1">
+        <v>43257</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
@@ -1359,13 +1376,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>

</xml_diff>